<commit_message>
up folder pkt moi 29/11
</commit_message>
<xml_diff>
--- a/Phòng kỹ thuật/Báo cáo/BÁO CÁO THÁNG 11/KPI/BÁO CÁO KPI/2. Xử lý các vấn đề Kỹ thuật/BẢNG CẬP NHẬT VÀ THEO DÕI CÁC VẤN ĐỀ PHÁT SING TRONG KÌ CẦN XỬ LÝ.xlsx
+++ b/Phòng kỹ thuật/Báo cáo/BÁO CÁO THÁNG 11/KPI/BÁO CÁO KPI/2. Xử lý các vấn đề Kỹ thuật/BẢNG CẬP NHẬT VÀ THEO DÕI CÁC VẤN ĐỀ PHÁT SING TRONG KÌ CẦN XỬ LÝ.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\kimhuong\Phòng kỹ thuật\Báo cáo\BÁO CÁO THÁNG 11\KPI\BÁO CÁO KPI\2. Xử lý các vấn đề Kỹ thuật\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B26830A-6051-4D79-92F4-9900922EC266}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8C9F01E-AB65-4965-9DE0-7522F20834B1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="106">
   <si>
     <t>STT</t>
   </si>
@@ -62,12 +62,6 @@
   </si>
   <si>
     <t>Viết danh sách các sản phẩm đã bán cho Huge Bamboo (tên sản phẩm, thành phần tên chất, nồng độ, số cas)</t>
-  </si>
-  <si>
-    <t>Tìm CTPT và số cas cho các chất theo yêu cầu của phòng tổng vụ:</t>
-  </si>
-  <si>
-    <t>10.1</t>
   </si>
   <si>
     <t>3.1</t>
@@ -187,9 +181,6 @@
     <t xml:space="preserve">BẢNG CẬP NHẬT CÁC VẤN ĐỀ PHÁT SING TRONG KÌ CẦN XỬ LÝ </t>
   </si>
   <si>
-    <t>Tìm CTPT và số cas cho các chất theo yêu cầu của phòng tổng vụ</t>
-  </si>
-  <si>
     <t>Xét xem sản phẩm SA-62 có đủ tiêu chuẩn làm chứng nhận OEKO-TEX không.</t>
   </si>
   <si>
@@ -232,15 +223,6 @@
     <t>3.13</t>
   </si>
   <si>
-    <t>3 phiếu</t>
-  </si>
-  <si>
-    <t>4 phiếu</t>
-  </si>
-  <si>
-    <t>5 phiếu</t>
-  </si>
-  <si>
     <t>H-71 (NCC08) Urea (HX)</t>
   </si>
   <si>
@@ -271,36 +253,12 @@
     <t>H-525 (NCC29) NP-915E (HX)</t>
   </si>
   <si>
-    <t>H-585</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H-583 </t>
-  </si>
-  <si>
-    <t>H-587</t>
-  </si>
-  <si>
-    <t>H-628</t>
-  </si>
-  <si>
     <t>H-339 (NCC06) Potassium persulfate (QX)</t>
   </si>
   <si>
     <t>Huntex OW-222</t>
   </si>
   <si>
-    <t>2.1</t>
-  </si>
-  <si>
-    <t>2.2</t>
-  </si>
-  <si>
-    <t>2.3</t>
-  </si>
-  <si>
-    <t>2.4</t>
-  </si>
-  <si>
     <t>4.1</t>
   </si>
   <si>
@@ -356,6 +314,92 @@
   </si>
   <si>
     <t>11.2</t>
+  </si>
+  <si>
+    <t>Viết tiêu chuẩn BS cho các chất cần đặt hàng:
+H-141 (Ablutex RTM), H-231 (Ablutex D600), H-233 (sinopol 1109).</t>
+  </si>
+  <si>
+    <t>9.16</t>
+  </si>
+  <si>
+    <t>Huntex UVP-222</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Làm nội dung trong nhãn sản phẩm </t>
+  </si>
+  <si>
+    <t>11.3</t>
+  </si>
+  <si>
+    <t>11.4</t>
+  </si>
+  <si>
+    <t>Huntex ITS-507 (H-507)</t>
+  </si>
+  <si>
+    <t>Huntex SLY-02 (HMBTSCT-07)</t>
+  </si>
+  <si>
+    <t>Dịch SDS cho phòng thu mua (PTM)</t>
+  </si>
+  <si>
+    <t>12.1</t>
+  </si>
+  <si>
+    <t>12.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R-330 AFINE (Chất tăng trắng huỳnh quang) </t>
+  </si>
+  <si>
+    <t>VN-UVITEX ER-RS (Chất tăng trắng huỳnh quang)</t>
+  </si>
+  <si>
+    <t>7.1</t>
+  </si>
+  <si>
+    <t>7.2</t>
+  </si>
+  <si>
+    <t>Benzyl benzoat</t>
+  </si>
+  <si>
+    <t>Tìm CTPT và số cas cho các chất theo yêu cầu của phòng thu mua:</t>
+  </si>
+  <si>
+    <t>Tìm CTPT và số cas cho các chất theo yêu cầu của phòng thu mua</t>
+  </si>
+  <si>
+    <t>H-583 (NCC29) SS-8380 (HX)</t>
+  </si>
+  <si>
+    <t>H-585 (NCC29) 3T-60 (HX)</t>
+  </si>
+  <si>
+    <t>H-587 (NCC29) 900 TYPE (HX)</t>
+  </si>
+  <si>
+    <t>H-628 (NCC29) NP-910A(30%) (HX)</t>
+  </si>
+  <si>
+    <t>Dịch SDS TA, TV cho phòng thu mua (PTM)</t>
+  </si>
+  <si>
+    <t>Giải quyết vấn đề kỹ thuật: Khách hàng Vĩnh Phương yêu cầu phải có chứng nhận ZDHC cho sản phẩm hồ sợi MB-115.</t>
+  </si>
+  <si>
+    <t>A.Quốc Minh</t>
+  </si>
+  <si>
+    <t>Đang thực hiện</t>
+  </si>
+  <si>
+    <t>S.Hùng</t>
+  </si>
+  <si>
+    <t>Tính nồng độ ppm của HCHO trong 1 kg sản phẩm
+CMHT-16</t>
   </si>
 </sst>
 </file>
@@ -419,7 +463,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -608,19 +652,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="hair">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -653,7 +684,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -705,9 +736,6 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -721,16 +749,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -745,12 +767,6 @@
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -763,6 +779,42 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -787,9 +839,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -814,13 +863,40 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -829,16 +905,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -850,23 +917,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1184,8 +1248,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F151"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -1197,49 +1261,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="45" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
+      <c r="A1" s="52" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
     </row>
     <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="47" t="s">
+      <c r="A3" s="45" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="45"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+    </row>
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="45" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+    </row>
+    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="47"/>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-    </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="47" t="s">
-        <v>28</v>
-      </c>
-      <c r="B4" s="47"/>
-      <c r="C4" s="47"/>
-      <c r="D4" s="47"/>
-      <c r="E4" s="47"/>
-    </row>
-    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="47" t="s">
-        <v>29</v>
-      </c>
-      <c r="B5" s="47"/>
-      <c r="C5" s="47"/>
-      <c r="D5" s="47"/>
-      <c r="E5" s="47"/>
+      <c r="B5" s="45"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="45"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
@@ -1252,75 +1316,75 @@
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="39" t="s">
+      <c r="B7" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="39"/>
+      <c r="C7" s="46"/>
       <c r="D7" s="12" t="s">
         <v>1</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>1</v>
       </c>
-      <c r="B8" s="40" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" s="40"/>
+      <c r="B8" s="47" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="47"/>
       <c r="D8" s="5">
         <v>44867</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>2</v>
       </c>
-      <c r="B9" s="41" t="s">
+      <c r="B9" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="41"/>
+      <c r="C9" s="48"/>
       <c r="D9" s="5">
         <v>44868</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="14">
         <v>3</v>
       </c>
-      <c r="B10" s="42" t="s">
+      <c r="B10" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="42"/>
+      <c r="C10" s="49"/>
       <c r="D10" s="13"/>
       <c r="E10" s="13" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="49">
+      <c r="A11" s="55">
         <v>4</v>
       </c>
-      <c r="B11" s="43" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="44"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="22"/>
+      <c r="B11" s="50" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="51"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="21"/>
     </row>
     <row r="12" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="50"/>
-      <c r="B12" s="30">
-        <v>4.0999999999999996</v>
+      <c r="A12" s="56"/>
+      <c r="B12" s="27" t="s">
+        <v>59</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>7</v>
@@ -1329,13 +1393,13 @@
         <v>44867</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="51"/>
-      <c r="B13" s="31">
-        <v>4.2</v>
+      <c r="A13" s="57"/>
+      <c r="B13" s="28" t="s">
+        <v>60</v>
       </c>
       <c r="C13" s="10" t="s">
         <v>8</v>
@@ -1344,188 +1408,213 @@
         <v>44870</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="F13" s="23"/>
+        <v>21</v>
+      </c>
+      <c r="F13" s="22"/>
     </row>
     <row r="14" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="21">
+      <c r="A14" s="20">
         <v>5</v>
       </c>
-      <c r="B14" s="52" t="s">
+      <c r="B14" s="58" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="53"/>
+      <c r="C14" s="59"/>
       <c r="D14" s="5">
         <v>44870</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F14" s="24"/>
+        <v>21</v>
+      </c>
+      <c r="F14" s="23"/>
     </row>
     <row r="15" spans="1:6" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>6</v>
       </c>
-      <c r="B15" s="52" t="s">
+      <c r="B15" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="53"/>
+      <c r="C15" s="59"/>
       <c r="D15" s="5">
         <v>44872</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F15" s="24"/>
+        <v>22</v>
+      </c>
+      <c r="F15" s="23"/>
     </row>
     <row r="16" spans="1:6" ht="30.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <v>7</v>
       </c>
-      <c r="B16" s="54" t="s">
-        <v>35</v>
-      </c>
-      <c r="C16" s="54"/>
+      <c r="B16" s="60" t="s">
+        <v>95</v>
+      </c>
+      <c r="C16" s="60"/>
       <c r="D16" s="4"/>
       <c r="E16" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="F16" s="24"/>
-    </row>
-    <row r="17" spans="1:5" ht="30.95" customHeight="1" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+      <c r="F16" s="23"/>
+    </row>
+    <row r="17" spans="1:6" ht="30.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="17">
         <v>8</v>
       </c>
-      <c r="B17" s="54" t="s">
-        <v>36</v>
-      </c>
-      <c r="C17" s="55"/>
+      <c r="B17" s="60" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="61"/>
       <c r="D17" s="5">
         <v>44881</v>
       </c>
       <c r="E17" s="17" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>9</v>
       </c>
-      <c r="B18" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="C18" s="48"/>
+      <c r="B18" s="54" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="54"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>10</v>
       </c>
-      <c r="B19" s="47" t="s">
-        <v>41</v>
-      </c>
-      <c r="C19" s="47"/>
+      <c r="B19" s="45" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="45"/>
       <c r="D19" s="5">
         <v>44881</v>
       </c>
       <c r="E19" s="3"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>11</v>
       </c>
-      <c r="B20" s="47" t="s">
-        <v>43</v>
-      </c>
-      <c r="C20" s="47"/>
-      <c r="D20" s="32"/>
+      <c r="B20" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="45"/>
+      <c r="D20" s="29"/>
       <c r="E20" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="44">
+        <v>12</v>
+      </c>
+      <c r="B21" s="45" t="s">
+        <v>86</v>
+      </c>
+      <c r="C21" s="45"/>
+      <c r="D21" s="36"/>
+      <c r="E21" s="36" t="s">
+        <v>20</v>
+      </c>
+      <c r="F21" s="36"/>
+    </row>
+    <row r="22" spans="1:6" ht="52.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="39">
+        <v>13</v>
+      </c>
+      <c r="B22" s="84" t="s">
+        <v>101</v>
+      </c>
+      <c r="C22" s="83"/>
+      <c r="D22" s="38">
+        <v>44894</v>
+      </c>
+      <c r="E22" s="39" t="s">
+        <v>102</v>
+      </c>
+      <c r="F22" s="39"/>
+    </row>
+    <row r="23" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="39">
+        <v>14</v>
+      </c>
+      <c r="B23" s="84" t="s">
+        <v>105</v>
+      </c>
+      <c r="C23" s="83"/>
+      <c r="D23" s="38">
+        <v>44894</v>
+      </c>
+      <c r="E23" s="39" t="s">
+        <v>104</v>
+      </c>
+      <c r="F23" s="40"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -2366,10 +2455,9 @@
       <c r="E151" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="18">
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
+  <mergeCells count="21">
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
     <mergeCell ref="A11:A13"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="B15:C15"/>
@@ -2380,11 +2468,15 @@
     <mergeCell ref="A3:E3"/>
     <mergeCell ref="A4:E4"/>
     <mergeCell ref="A5:E5"/>
+    <mergeCell ref="B21:C21"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2393,70 +2485,70 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F184"/>
+  <dimension ref="A1:F182"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B55" sqref="B55"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D59" sqref="D59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="5.33203125" customWidth="1"/>
-    <col min="3" max="3" width="38.109375" customWidth="1"/>
+    <col min="3" max="3" width="39" customWidth="1"/>
     <col min="4" max="4" width="14" style="1" customWidth="1"/>
     <col min="5" max="5" width="17.6640625" style="1" customWidth="1"/>
     <col min="6" max="6" width="14.33203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="45" t="s">
-        <v>37</v>
-      </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
+      <c r="A1" s="52" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
     </row>
     <row r="2" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
     </row>
     <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="47" t="s">
+      <c r="A3" s="45" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="45"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="45"/>
+    </row>
+    <row r="4" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="45" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="47"/>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47"/>
-    </row>
-    <row r="4" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="47" t="s">
-        <v>28</v>
-      </c>
-      <c r="B4" s="47"/>
-      <c r="C4" s="47"/>
-      <c r="D4" s="47"/>
-      <c r="E4" s="47"/>
-      <c r="F4" s="47"/>
-    </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="47" t="s">
-        <v>29</v>
-      </c>
-      <c r="B5" s="47"/>
-      <c r="C5" s="47"/>
-      <c r="D5" s="47"/>
-      <c r="E5" s="47"/>
-      <c r="F5" s="47"/>
+      <c r="B5" s="45"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="45"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
@@ -2470,15 +2562,15 @@
       <c r="A7" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="39" t="s">
+      <c r="B7" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="39"/>
+      <c r="C7" s="46"/>
       <c r="D7" s="18" t="s">
         <v>1</v>
       </c>
       <c r="E7" s="18" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F7" s="18" t="s">
         <v>10</v>
@@ -2488,748 +2580,762 @@
       <c r="A8" s="17">
         <v>1</v>
       </c>
-      <c r="B8" s="40" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" s="40"/>
+      <c r="B8" s="47" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="47"/>
       <c r="D8" s="5">
         <v>44867</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F8" s="17" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="49">
+    <row r="9" spans="1:6" ht="48.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="33">
         <v>2</v>
       </c>
-      <c r="B9" s="41" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" s="41"/>
-      <c r="D9" s="5"/>
+      <c r="B9" s="47" t="s">
+        <v>78</v>
+      </c>
+      <c r="C9" s="48"/>
+      <c r="D9" s="5">
+        <v>44890</v>
+      </c>
       <c r="E9" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F9" s="17" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="50"/>
-      <c r="B10" s="25" t="s">
-        <v>69</v>
-      </c>
-      <c r="C10" s="33"/>
-      <c r="D10" s="34"/>
-      <c r="E10" s="34"/>
-      <c r="F10" s="25"/>
+      <c r="A10" s="74">
+        <v>3</v>
+      </c>
+      <c r="B10" s="49" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="49"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="67" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="55" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="50"/>
+      <c r="A11" s="75"/>
       <c r="B11" s="25" t="s">
-        <v>70</v>
-      </c>
-      <c r="C11" s="33"/>
-      <c r="D11" s="34"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="25"/>
+        <v>12</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="8">
+        <v>44866</v>
+      </c>
+      <c r="E11" s="68"/>
+      <c r="F11" s="56"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="50"/>
-      <c r="B12" s="38" t="s">
-        <v>71</v>
-      </c>
-      <c r="C12" s="33"/>
-      <c r="D12" s="34"/>
-      <c r="E12" s="34"/>
-      <c r="F12" s="25"/>
+      <c r="A12" s="75"/>
+      <c r="B12" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="8">
+        <v>44868</v>
+      </c>
+      <c r="E12" s="68"/>
+      <c r="F12" s="56"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="51"/>
-      <c r="B13" s="38" t="s">
-        <v>72</v>
-      </c>
-      <c r="C13" s="33"/>
-      <c r="D13" s="34"/>
-      <c r="E13" s="34"/>
-      <c r="F13" s="25"/>
+      <c r="A13" s="75"/>
+      <c r="B13" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="8">
+        <v>44869</v>
+      </c>
+      <c r="E13" s="68"/>
+      <c r="F13" s="56"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="59">
-        <v>3</v>
-      </c>
-      <c r="B14" s="42" t="s">
+      <c r="A14" s="75"/>
+      <c r="B14" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="8">
+        <v>44872</v>
+      </c>
+      <c r="E14" s="68"/>
+      <c r="F14" s="56"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="75"/>
+      <c r="B15" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="8">
+        <v>44873</v>
+      </c>
+      <c r="E15" s="68"/>
+      <c r="F15" s="56"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="73"/>
+      <c r="B16" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" s="19">
+        <v>44875</v>
+      </c>
+      <c r="E16" s="68"/>
+      <c r="F16" s="56"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="73"/>
+      <c r="B17" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" s="19">
+        <v>44879</v>
+      </c>
+      <c r="E17" s="68"/>
+      <c r="F17" s="56"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="73"/>
+      <c r="B18" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" s="19">
+        <v>44880</v>
+      </c>
+      <c r="E18" s="68"/>
+      <c r="F18" s="56"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="73"/>
+      <c r="B19" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" s="19">
+        <v>44882</v>
+      </c>
+      <c r="E19" s="68"/>
+      <c r="F19" s="56"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="73"/>
+      <c r="B20" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D20" s="19">
+        <v>44886</v>
+      </c>
+      <c r="E20" s="68"/>
+      <c r="F20" s="56"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="73"/>
+      <c r="B21" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D21" s="19">
+        <v>44888</v>
+      </c>
+      <c r="E21" s="68"/>
+      <c r="F21" s="56"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="73"/>
+      <c r="B22" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D22" s="35">
+        <v>44891</v>
+      </c>
+      <c r="E22" s="68"/>
+      <c r="F22" s="56"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="76"/>
+      <c r="B23" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D23" s="35">
+        <v>44893</v>
+      </c>
+      <c r="E23" s="69"/>
+      <c r="F23" s="57"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" s="77">
+        <v>4</v>
+      </c>
+      <c r="B24" s="78" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" s="78"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="14"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="77"/>
+      <c r="B25" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" s="8">
+        <v>44867</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F25" s="15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="33" x14ac:dyDescent="0.3">
+      <c r="A26" s="77"/>
+      <c r="B26" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D26" s="11">
+        <v>44870</v>
+      </c>
+      <c r="E26" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F26" s="16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="17">
         <v>5</v>
       </c>
-      <c r="C14" s="42"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="60"/>
-      <c r="B15" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D15" s="8">
-        <v>44866</v>
-      </c>
-      <c r="E15" s="56" t="s">
-        <v>24</v>
-      </c>
-      <c r="F15" s="15" t="s">
+      <c r="B27" s="60" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27" s="60"/>
+      <c r="D27" s="5">
+        <v>44870</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F27" s="17" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="60"/>
-      <c r="B16" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="C16" s="7" t="s">
+    <row r="28" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="17">
+        <v>6</v>
+      </c>
+      <c r="B28" s="60" t="s">
+        <v>11</v>
+      </c>
+      <c r="C28" s="60"/>
+      <c r="D28" s="5">
+        <v>44872</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F28" s="17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="39" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="17">
+        <v>7</v>
+      </c>
+      <c r="B29" s="79" t="s">
+        <v>94</v>
+      </c>
+      <c r="C29" s="79"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="14"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" s="6"/>
+      <c r="B30" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="C30" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D16" s="8">
-        <v>44868</v>
-      </c>
-      <c r="E16" s="57"/>
-      <c r="F16" s="15" t="s">
+      <c r="D30" s="11">
+        <v>44873</v>
+      </c>
+      <c r="E30" s="73" t="s">
+        <v>20</v>
+      </c>
+      <c r="F30" s="73" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="60"/>
-      <c r="B17" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D17" s="8">
-        <v>44869</v>
-      </c>
-      <c r="E17" s="57"/>
-      <c r="F17" s="15" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="60"/>
-      <c r="B18" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D18" s="8">
-        <v>44872</v>
-      </c>
-      <c r="E18" s="57"/>
-      <c r="F18" s="15" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="60"/>
-      <c r="B19" s="27" t="s">
-        <v>25</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D19" s="8">
-        <v>44873</v>
-      </c>
-      <c r="E19" s="57"/>
-      <c r="F19" s="15" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="61"/>
-      <c r="B20" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D20" s="20">
-        <v>44875</v>
-      </c>
-      <c r="E20" s="57"/>
-      <c r="F20" s="15" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="61"/>
-      <c r="B21" s="27" t="s">
-        <v>32</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D21" s="20">
-        <v>44879</v>
-      </c>
-      <c r="E21" s="57"/>
-      <c r="F21" s="15" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="61"/>
-      <c r="B22" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D22" s="20">
-        <v>44880</v>
-      </c>
-      <c r="E22" s="57"/>
-      <c r="F22" s="27" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="61"/>
-      <c r="B23" s="27" t="s">
-        <v>45</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="D23" s="20">
-        <v>44882</v>
-      </c>
-      <c r="E23" s="57"/>
-      <c r="F23" s="27" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="61"/>
-      <c r="B24" s="27" t="s">
-        <v>46</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D24" s="20">
-        <v>44886</v>
-      </c>
-      <c r="E24" s="57"/>
-      <c r="F24" s="27" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" s="61"/>
-      <c r="B25" s="27" t="s">
-        <v>47</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="D25" s="20">
-        <v>44888</v>
-      </c>
-      <c r="E25" s="58"/>
-      <c r="F25" s="27" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="61"/>
-      <c r="B26" s="27" t="s">
-        <v>48</v>
-      </c>
-      <c r="C26" s="19"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="20"/>
-      <c r="F26" s="28"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27" s="62"/>
-      <c r="B27" s="27" t="s">
-        <v>49</v>
-      </c>
-      <c r="C27" s="9"/>
-      <c r="D27" s="16"/>
-      <c r="E27" s="16"/>
-      <c r="F27" s="16"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28" s="65">
-        <v>4</v>
-      </c>
-      <c r="B28" s="66" t="s">
-        <v>20</v>
-      </c>
-      <c r="C28" s="66"/>
-      <c r="D28" s="14"/>
-      <c r="E28" s="14"/>
-      <c r="F28" s="14"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29" s="65"/>
-      <c r="B29" s="27" t="s">
-        <v>73</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D29" s="8">
-        <v>44867</v>
-      </c>
-      <c r="E29" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="F29" s="15" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="33" x14ac:dyDescent="0.3">
-      <c r="A30" s="65"/>
-      <c r="B30" s="29" t="s">
-        <v>74</v>
-      </c>
-      <c r="C30" s="10" t="s">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" s="6"/>
+      <c r="B31" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="C31" s="41" t="s">
+        <v>93</v>
+      </c>
+      <c r="D31" s="42">
+        <v>44893</v>
+      </c>
+      <c r="E31" s="57"/>
+      <c r="F31" s="57"/>
+    </row>
+    <row r="32" spans="1:6" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="17">
         <v>8</v>
       </c>
-      <c r="D30" s="11">
-        <v>44870</v>
-      </c>
-      <c r="E30" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="F30" s="16" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="17">
-        <v>5</v>
-      </c>
-      <c r="B31" s="54" t="s">
-        <v>9</v>
-      </c>
-      <c r="C31" s="54"/>
-      <c r="D31" s="5">
-        <v>44870</v>
-      </c>
-      <c r="E31" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F31" s="17" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="17">
-        <v>6</v>
-      </c>
-      <c r="B32" s="54" t="s">
-        <v>11</v>
-      </c>
-      <c r="C32" s="54"/>
+      <c r="B32" s="60" t="s">
+        <v>33</v>
+      </c>
+      <c r="C32" s="61"/>
       <c r="D32" s="5">
-        <v>44872</v>
-      </c>
-      <c r="E32" s="5" t="s">
+        <v>44881</v>
+      </c>
+      <c r="E32" s="17" t="s">
         <v>24</v>
       </c>
       <c r="F32" s="17" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="39.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="17">
-        <v>7</v>
-      </c>
-      <c r="B33" s="67" t="s">
-        <v>12</v>
-      </c>
-      <c r="C33" s="67"/>
-      <c r="D33" s="14"/>
-      <c r="E33" s="14"/>
-      <c r="F33" s="14"/>
-    </row>
-    <row r="34" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="6"/>
-      <c r="B34" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="C34" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="D34" s="11">
-        <v>44873</v>
-      </c>
-      <c r="E34" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="F34" s="16" t="s">
+    <row r="33" spans="1:6" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="65">
+        <v>9</v>
+      </c>
+      <c r="B33" s="54" t="s">
+        <v>36</v>
+      </c>
+      <c r="C33" s="54"/>
+      <c r="D33" s="3"/>
+      <c r="F33" s="3"/>
+    </row>
+    <row r="34" spans="1:6" ht="39.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="64"/>
+      <c r="B34" s="32" t="s">
+        <v>61</v>
+      </c>
+      <c r="C34" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="D34" s="5">
+        <v>44882</v>
+      </c>
+      <c r="E34" s="71" t="s">
+        <v>37</v>
+      </c>
+      <c r="F34" s="55" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="17">
-        <v>8</v>
-      </c>
-      <c r="B35" s="54" t="s">
-        <v>36</v>
-      </c>
-      <c r="C35" s="55"/>
-      <c r="D35" s="5">
-        <v>44881</v>
-      </c>
-      <c r="E35" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="F35" s="17" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="63">
-        <v>9</v>
-      </c>
-      <c r="B36" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="C36" s="48"/>
-      <c r="D36" s="3"/>
-      <c r="F36" s="3"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="64"/>
+      <c r="B35" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="C35" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="D35" s="80">
+        <v>44883</v>
+      </c>
+      <c r="E35" s="72"/>
+      <c r="F35" s="56"/>
+    </row>
+    <row r="36" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="64"/>
+      <c r="B36" s="32" t="s">
+        <v>63</v>
+      </c>
+      <c r="C36" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="D36" s="81"/>
+      <c r="E36" s="72"/>
+      <c r="F36" s="56"/>
+    </row>
+    <row r="37" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="64"/>
-      <c r="B37" s="37" t="s">
-        <v>75</v>
-      </c>
-      <c r="C37" s="36" t="s">
-        <v>67</v>
-      </c>
-      <c r="D37" s="5">
-        <v>44882</v>
-      </c>
-      <c r="E37" s="68" t="s">
-        <v>40</v>
-      </c>
-      <c r="F37" s="26" t="s">
-        <v>6</v>
-      </c>
+      <c r="B37" s="32" t="s">
+        <v>64</v>
+      </c>
+      <c r="C37" s="30" t="s">
+        <v>49</v>
+      </c>
+      <c r="D37" s="81"/>
+      <c r="E37" s="72"/>
+      <c r="F37" s="56"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="64"/>
-      <c r="B38" s="37" t="s">
-        <v>76</v>
-      </c>
-      <c r="C38" s="35" t="s">
-        <v>53</v>
-      </c>
-      <c r="D38" s="71">
-        <v>44883</v>
-      </c>
-      <c r="E38" s="69"/>
-      <c r="F38" s="26" t="s">
-        <v>6</v>
-      </c>
+      <c r="B38" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="C38" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="D38" s="81"/>
+      <c r="E38" s="72"/>
+      <c r="F38" s="56"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="64"/>
-      <c r="B39" s="37" t="s">
-        <v>77</v>
-      </c>
-      <c r="C39" s="35" t="s">
-        <v>54</v>
-      </c>
-      <c r="D39" s="72"/>
-      <c r="E39" s="69"/>
-      <c r="F39" s="26" t="s">
-        <v>6</v>
-      </c>
+      <c r="B39" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="C39" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="D39" s="81"/>
+      <c r="E39" s="72"/>
+      <c r="F39" s="56"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="64"/>
-      <c r="B40" s="37" t="s">
-        <v>78</v>
-      </c>
-      <c r="C40" s="35" t="s">
-        <v>55</v>
-      </c>
-      <c r="D40" s="72"/>
-      <c r="E40" s="69"/>
-      <c r="F40" s="26" t="s">
-        <v>6</v>
-      </c>
+      <c r="B40" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="C40" s="30" t="s">
+        <v>52</v>
+      </c>
+      <c r="D40" s="70">
+        <v>44884</v>
+      </c>
+      <c r="E40" s="72"/>
+      <c r="F40" s="56"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="64"/>
-      <c r="B41" s="37" t="s">
-        <v>79</v>
-      </c>
-      <c r="C41" s="35" t="s">
-        <v>56</v>
-      </c>
-      <c r="D41" s="72"/>
-      <c r="E41" s="69"/>
-      <c r="F41" s="26" t="s">
-        <v>6</v>
-      </c>
+      <c r="B41" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="C41" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="D41" s="70"/>
+      <c r="E41" s="72"/>
+      <c r="F41" s="56"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="64"/>
-      <c r="B42" s="37" t="s">
-        <v>80</v>
-      </c>
-      <c r="C42" s="35" t="s">
-        <v>57</v>
-      </c>
-      <c r="D42" s="72"/>
-      <c r="E42" s="69"/>
-      <c r="F42" s="26" t="s">
-        <v>6</v>
-      </c>
+      <c r="B42" s="32" t="s">
+        <v>69</v>
+      </c>
+      <c r="C42" s="30" t="s">
+        <v>54</v>
+      </c>
+      <c r="D42" s="70"/>
+      <c r="E42" s="72"/>
+      <c r="F42" s="56"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="64"/>
-      <c r="B43" s="37" t="s">
-        <v>81</v>
-      </c>
-      <c r="C43" s="35" t="s">
-        <v>58</v>
-      </c>
-      <c r="D43" s="70">
-        <v>44884</v>
-      </c>
-      <c r="E43" s="69"/>
-      <c r="F43" s="26" t="s">
-        <v>6</v>
-      </c>
+      <c r="B43" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="C43" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="D43" s="29">
+        <v>44886</v>
+      </c>
+      <c r="E43" s="72"/>
+      <c r="F43" s="56"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="64"/>
-      <c r="B44" s="37" t="s">
-        <v>82</v>
-      </c>
-      <c r="C44" s="35" t="s">
-        <v>59</v>
-      </c>
-      <c r="D44" s="70"/>
-      <c r="E44" s="69"/>
-      <c r="F44" s="26" t="s">
-        <v>6</v>
-      </c>
+      <c r="B44" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="C44" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="D44" s="29">
+        <v>44889</v>
+      </c>
+      <c r="E44" s="72"/>
+      <c r="F44" s="56"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="64"/>
-      <c r="B45" s="37" t="s">
-        <v>83</v>
-      </c>
-      <c r="C45" s="35" t="s">
-        <v>60</v>
-      </c>
-      <c r="D45" s="70"/>
-      <c r="E45" s="69"/>
-      <c r="F45" s="26" t="s">
-        <v>6</v>
-      </c>
+      <c r="B45" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="C45" s="30" t="s">
+        <v>96</v>
+      </c>
+      <c r="D45" s="70">
+        <v>44890</v>
+      </c>
+      <c r="E45" s="72"/>
+      <c r="F45" s="56"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="64"/>
-      <c r="B46" s="37" t="s">
-        <v>84</v>
-      </c>
-      <c r="C46" s="35" t="s">
-        <v>61</v>
-      </c>
-      <c r="D46" s="32">
-        <v>44886</v>
-      </c>
-      <c r="E46" s="69"/>
-      <c r="F46" s="26" t="s">
-        <v>6</v>
-      </c>
+      <c r="B46" s="32" t="s">
+        <v>73</v>
+      </c>
+      <c r="C46" s="30" t="s">
+        <v>97</v>
+      </c>
+      <c r="D46" s="70"/>
+      <c r="E46" s="72"/>
+      <c r="F46" s="56"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="64"/>
-      <c r="B47" s="37" t="s">
-        <v>85</v>
-      </c>
-      <c r="C47" s="35" t="s">
-        <v>62</v>
-      </c>
-      <c r="D47" s="32">
-        <v>44889</v>
-      </c>
-      <c r="E47" s="69"/>
-      <c r="F47" s="26" t="s">
-        <v>6</v>
-      </c>
+      <c r="B47" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="C47" s="30" t="s">
+        <v>98</v>
+      </c>
+      <c r="D47" s="70"/>
+      <c r="E47" s="72"/>
+      <c r="F47" s="56"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="64"/>
-      <c r="B48" s="37" t="s">
-        <v>86</v>
-      </c>
-      <c r="C48" s="35" t="s">
-        <v>64</v>
-      </c>
-      <c r="D48" s="70"/>
-      <c r="E48" s="69"/>
-      <c r="F48" s="26" t="s">
+      <c r="B48" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="C48" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="D48" s="82"/>
+      <c r="E48" s="72"/>
+      <c r="F48" s="56"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A49" s="36"/>
+      <c r="B49" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="C49" s="30" t="s">
+        <v>52</v>
+      </c>
+      <c r="D49" s="37">
+        <v>44893</v>
+      </c>
+      <c r="E49" s="72"/>
+      <c r="F49" s="57"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A50" s="3">
+        <v>10</v>
+      </c>
+      <c r="B50" s="45" t="s">
+        <v>38</v>
+      </c>
+      <c r="C50" s="45"/>
+      <c r="D50" s="5">
+        <v>44881</v>
+      </c>
+      <c r="E50" s="3"/>
+      <c r="F50" s="24" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A49" s="64"/>
-      <c r="B49" s="37" t="s">
-        <v>87</v>
-      </c>
-      <c r="C49" s="35" t="s">
-        <v>63</v>
-      </c>
-      <c r="D49" s="70"/>
-      <c r="E49" s="69"/>
-      <c r="F49" s="26" t="s">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A51" s="3">
+        <v>11</v>
+      </c>
+      <c r="B51" s="45" t="s">
+        <v>81</v>
+      </c>
+      <c r="C51" s="45"/>
+      <c r="D51" s="29"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A52" s="2"/>
+      <c r="B52" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D52" s="70">
+        <v>44886</v>
+      </c>
+      <c r="E52" s="66" t="s">
+        <v>39</v>
+      </c>
+      <c r="F52" s="65" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A50" s="64"/>
-      <c r="B50" s="37" t="s">
-        <v>88</v>
-      </c>
-      <c r="C50" s="35" t="s">
-        <v>65</v>
-      </c>
-      <c r="D50" s="70"/>
-      <c r="E50" s="69"/>
-      <c r="F50" s="26" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A51" s="64"/>
-      <c r="B51" s="37" t="s">
-        <v>89</v>
-      </c>
-      <c r="C51" s="35" t="s">
-        <v>66</v>
-      </c>
-      <c r="D51" s="73"/>
-      <c r="E51" s="69"/>
-      <c r="F51" s="26" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A52" s="3">
-        <v>10</v>
-      </c>
-      <c r="B52" s="47" t="s">
-        <v>41</v>
-      </c>
-      <c r="C52" s="47"/>
-      <c r="D52" s="5">
-        <v>44881</v>
-      </c>
-      <c r="E52" s="3"/>
-      <c r="F52" s="26" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="3">
-        <v>11</v>
-      </c>
-      <c r="B53" s="47" t="s">
-        <v>43</v>
-      </c>
-      <c r="C53" s="47"/>
-      <c r="D53" s="32"/>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A53" s="2"/>
+      <c r="B53" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D53" s="70"/>
+      <c r="E53" s="66"/>
+      <c r="F53" s="66"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" s="2"/>
-      <c r="B54" s="3" t="s">
-        <v>90</v>
+      <c r="B54" s="36" t="s">
+        <v>82</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>68</v>
+        <v>84</v>
       </c>
       <c r="D54" s="70">
-        <v>44886</v>
-      </c>
-      <c r="E54" s="69" t="s">
-        <v>42</v>
-      </c>
-      <c r="F54" s="26" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+        <v>44890</v>
+      </c>
+      <c r="E54" s="66"/>
+      <c r="F54" s="66"/>
+    </row>
+    <row r="55" spans="1:6" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="2"/>
-      <c r="B55" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>68</v>
+      <c r="B55" s="36" t="s">
+        <v>83</v>
+      </c>
+      <c r="C55" s="43" t="s">
+        <v>85</v>
       </c>
       <c r="D55" s="70"/>
-      <c r="E55" s="69"/>
-      <c r="F55" s="26" t="s">
-        <v>6</v>
-      </c>
+      <c r="E55" s="66"/>
+      <c r="F55" s="66"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A56" s="2"/>
-      <c r="B56" s="2"/>
-      <c r="C56" s="2"/>
+      <c r="A56" s="44">
+        <v>12</v>
+      </c>
+      <c r="B56" s="45" t="s">
+        <v>100</v>
+      </c>
+      <c r="C56" s="45"/>
       <c r="D56" s="3"/>
       <c r="E56" s="3"/>
       <c r="F56" s="3"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" s="2"/>
-      <c r="B57" s="2"/>
-      <c r="C57" s="2"/>
-      <c r="D57" s="3"/>
-      <c r="E57" s="3"/>
-      <c r="F57" s="3"/>
+      <c r="B57" s="36" t="s">
+        <v>87</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D57" s="62">
+        <v>44893</v>
+      </c>
+      <c r="E57" s="64" t="s">
+        <v>20</v>
+      </c>
+      <c r="F57" s="65" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" s="2"/>
-      <c r="B58" s="2"/>
-      <c r="C58" s="2"/>
-      <c r="D58" s="3"/>
-      <c r="E58" s="3"/>
-      <c r="F58" s="3"/>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A59" s="2"/>
-      <c r="B59" s="2"/>
-      <c r="C59" s="2"/>
-      <c r="D59" s="3"/>
-      <c r="E59" s="3"/>
-      <c r="F59" s="3"/>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A60" s="2"/>
-      <c r="B60" s="2"/>
-      <c r="C60" s="2"/>
-      <c r="D60" s="3"/>
-      <c r="E60" s="3"/>
-      <c r="F60" s="3"/>
+      <c r="B58" s="36" t="s">
+        <v>88</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D58" s="63"/>
+      <c r="E58" s="64"/>
+      <c r="F58" s="66"/>
+    </row>
+    <row r="59" spans="1:6" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="39">
+        <v>13</v>
+      </c>
+      <c r="B59" s="84" t="s">
+        <v>101</v>
+      </c>
+      <c r="C59" s="83"/>
+      <c r="D59" s="38">
+        <v>44894</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="F59" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="39">
+        <v>14</v>
+      </c>
+      <c r="B60" s="84" t="s">
+        <v>105</v>
+      </c>
+      <c r="C60" s="83"/>
+      <c r="D60" s="38">
+        <v>44894</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="F60" s="40" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" s="2"/>
@@ -4207,52 +4313,47 @@
       <c r="E182" s="3"/>
       <c r="F182" s="3"/>
     </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A183" s="2"/>
-      <c r="B183" s="2"/>
-      <c r="C183" s="2"/>
-      <c r="D183" s="3"/>
-      <c r="E183" s="3"/>
-      <c r="F183" s="3"/>
-    </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A184" s="2"/>
-      <c r="B184" s="2"/>
-      <c r="C184" s="2"/>
-      <c r="D184" s="3"/>
-      <c r="E184" s="3"/>
-      <c r="F184" s="3"/>
-    </row>
   </sheetData>
-  <mergeCells count="28">
-    <mergeCell ref="E37:E51"/>
-    <mergeCell ref="E54:E55"/>
-    <mergeCell ref="D54:D55"/>
-    <mergeCell ref="D38:D42"/>
-    <mergeCell ref="D43:D45"/>
-    <mergeCell ref="D48:D51"/>
-    <mergeCell ref="A36:A51"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="A9:A13"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="A28:A30"/>
+  <mergeCells count="39">
+    <mergeCell ref="D45:D48"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="A24:A26"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B27:C27"/>
     <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="A33:A48"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B51:C51"/>
     <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B33:C33"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A3:F3"/>
     <mergeCell ref="A4:F4"/>
     <mergeCell ref="A5:F5"/>
-    <mergeCell ref="E15:E25"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="B9:C9"/>
-    <mergeCell ref="A14:A27"/>
-    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="A10:A23"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="D57:D58"/>
+    <mergeCell ref="E57:E58"/>
+    <mergeCell ref="F57:F58"/>
+    <mergeCell ref="E10:E23"/>
+    <mergeCell ref="F10:F23"/>
+    <mergeCell ref="D54:D55"/>
+    <mergeCell ref="E52:E55"/>
+    <mergeCell ref="F52:F55"/>
+    <mergeCell ref="F34:F49"/>
+    <mergeCell ref="E34:E49"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="F30:F31"/>
+    <mergeCell ref="D52:D53"/>
+    <mergeCell ref="D35:D39"/>
+    <mergeCell ref="D40:D42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>